<commit_message>
por fin 24 horas despues
</commit_message>
<xml_diff>
--- a/Modelos/Experimentos TFP y STL/Resultados.xlsx
+++ b/Modelos/Experimentos TFP y STL/Resultados.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/jd_pradal_uniandes_edu_co/Documents/Documentos/Maestría/Tesis Maestría/Modelos/Experimentos TFP y STL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{34A74DC2-6BF4-4ADA-A2A7-7E00B2D7711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DDA0984-CDBD-4B85-A35D-CB724FB5985C}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{34A74DC2-6BF4-4ADA-A2A7-7E00B2D7711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2EC8795-4D31-4577-B055-587770D9D661}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A9FAACA8-E109-4398-B007-65978125D358}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Temperatura Contugas" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="57">
   <si>
     <t>Nodos 1</t>
   </si>
@@ -114,16 +115,115 @@
   </si>
   <si>
     <t>STL_DP con epsilon0.01 Modelo 100 - nodos1 - 100 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 100 - nodos1 - 100 - nodos2 - 75 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 100 - nodos1 - 100 - nodos2 - 75 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 100 - nodos1 - 100 - nodos2 - 75 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 10 - nodos1 - 10 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 10 - nodos1 - 10 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 10 - nodos1 - 10 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 10 - nodos1 - 50 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 10 - nodos1 - 50 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 10 - nodos1 - 50 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 10 - nodos1 - 120 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 10 - nodos1 - 120 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 50 - nodos1 - 10 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 50 - nodos1 - 50 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 10 - nodos1 - 120 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 50 - nodos1 - 50 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 50 - nodos1 - 10 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 50 - nodos1 - 10 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 50 - nodos1 - 50 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 50 - nodos1 - 120 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 50 - nodos1 - 120 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 50 - nodos1 - 120 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 120 - nodos1 - 10 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 120 - nodos1 - 10 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 120 - nodos1 - 10 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 120 - nodos1 - 50 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 120 - nodos1 - 50 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 120 - nodos1 - 50 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>STL_DP con epsilon0.01 Modelo 120 - nodos1 - 120 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Sin ruido Modelo 120 - nodos1 - 120 - nodos2 - 50 Epocas 30 Batch</t>
+  </si>
+  <si>
+    <t>Contugas TFP Modelo 120 - nodos1 - 120 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -488,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE0AF1F-A591-4C48-994B-136B6B689247}">
-  <dimension ref="A3:L25"/>
+  <dimension ref="A3:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,70 +802,212 @@
       <c r="K8" t="s">
         <v>12</v>
       </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0.01</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0.01</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0.01</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="A12">
+        <v>0.01</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>30</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" t="s">
-        <v>4</v>
+      <c r="A13">
+        <v>0.01</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K13" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="L13" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
-        <f>1/100</f>
         <v>0.01</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C14">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -789,22 +1031,21 @@
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
-        <f>1/100</f>
         <v>0.01</v>
       </c>
       <c r="B15">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C15">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E15">
         <v>30</v>
@@ -828,19 +1069,18 @@
         <v>12</v>
       </c>
       <c r="L15" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
-        <f>1/100</f>
         <v>0.01</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C16">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D16">
         <v>50</v>
@@ -867,22 +1107,21 @@
         <v>12</v>
       </c>
       <c r="L16" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
-        <f>1/100</f>
         <v>0.01</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D17">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E17">
         <v>30</v>
@@ -905,133 +1144,58 @@
       <c r="K17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="L17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>0</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
         <v>4</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>5</v>
       </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
         <v>6</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J23" t="s">
         <v>7</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K23" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <f>1/100</f>
-        <v>0.01</v>
-      </c>
-      <c r="B22">
-        <v>100</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
-      <c r="E22">
-        <v>30</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" t="s">
-        <v>12</v>
-      </c>
-      <c r="L22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <f>1/100</f>
-        <v>0.01</v>
-      </c>
-      <c r="B23">
-        <v>100</v>
-      </c>
-      <c r="C23">
-        <v>100</v>
-      </c>
-      <c r="D23">
-        <v>20</v>
-      </c>
-      <c r="E23">
-        <v>30</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" t="s">
-        <v>12</v>
-      </c>
-      <c r="L23" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -1046,7 +1210,7 @@
         <v>100</v>
       </c>
       <c r="D24">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>30</v>
@@ -1070,7 +1234,7 @@
         <v>12</v>
       </c>
       <c r="L24" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -1085,36 +1249,1020 @@
         <v>100</v>
       </c>
       <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>30</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27">
         <v>75</v>
       </c>
-      <c r="E25">
-        <v>30</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-      <c r="I25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" t="s">
-        <v>12</v>
+      <c r="E27">
+        <v>30</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0.01</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>50</v>
+      </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0.01</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>50</v>
+      </c>
+      <c r="D29">
+        <v>50</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.01</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>120</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0.01</v>
+      </c>
+      <c r="B31">
+        <v>50</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>50</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0.01</v>
+      </c>
+      <c r="B32">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>50</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0.01</v>
+      </c>
+      <c r="B33">
+        <v>50</v>
+      </c>
+      <c r="C33">
+        <v>120</v>
+      </c>
+      <c r="D33">
+        <v>50</v>
+      </c>
+      <c r="E33">
+        <v>30</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0.01</v>
+      </c>
+      <c r="B34">
+        <v>120</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>50</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>0.01</v>
+      </c>
+      <c r="B35">
+        <v>120</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>50</v>
+      </c>
+      <c r="E35">
+        <v>30</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>0.01</v>
+      </c>
+      <c r="B36">
+        <v>120</v>
+      </c>
+      <c r="C36">
+        <v>120</v>
+      </c>
+      <c r="D36">
+        <v>50</v>
+      </c>
+      <c r="E36">
+        <v>30</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B41">
+        <v>100</v>
+      </c>
+      <c r="C41">
+        <v>100</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>30</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>11</v>
+      </c>
+      <c r="J41" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B42">
+        <v>100</v>
+      </c>
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>30</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B43">
+        <v>100</v>
+      </c>
+      <c r="C43">
+        <v>100</v>
+      </c>
+      <c r="D43">
+        <v>50</v>
+      </c>
+      <c r="E43">
+        <v>30</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>12</v>
+      </c>
+      <c r="K43" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B44">
+        <v>100</v>
+      </c>
+      <c r="C44">
+        <v>100</v>
+      </c>
+      <c r="D44">
+        <v>75</v>
+      </c>
+      <c r="E44">
+        <v>30</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" t="s">
+        <v>12</v>
+      </c>
+      <c r="L44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>0.01</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>50</v>
+      </c>
+      <c r="E45">
+        <v>30</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>0.01</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
+      </c>
+      <c r="D46">
+        <v>50</v>
+      </c>
+      <c r="E46">
+        <v>30</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>0.01</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>120</v>
+      </c>
+      <c r="D47">
+        <v>50</v>
+      </c>
+      <c r="E47">
+        <v>30</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>0.01</v>
+      </c>
+      <c r="B48">
+        <v>50</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>50</v>
+      </c>
+      <c r="E48">
+        <v>30</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48">
+        <v>3</v>
+      </c>
+      <c r="I48" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" t="s">
+        <v>12</v>
+      </c>
+      <c r="K48" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>0.01</v>
+      </c>
+      <c r="B49">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <v>50</v>
+      </c>
+      <c r="E49">
+        <v>30</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49">
+        <v>3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49" t="s">
+        <v>12</v>
+      </c>
+      <c r="L49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>0.01</v>
+      </c>
+      <c r="B50">
+        <v>50</v>
+      </c>
+      <c r="C50">
+        <v>120</v>
+      </c>
+      <c r="D50">
+        <v>50</v>
+      </c>
+      <c r="E50">
+        <v>30</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" t="s">
+        <v>12</v>
+      </c>
+      <c r="K50" t="s">
+        <v>12</v>
+      </c>
+      <c r="L50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>0.01</v>
+      </c>
+      <c r="B51">
+        <v>120</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>50</v>
+      </c>
+      <c r="E51">
+        <v>30</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+      <c r="I51" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>0.01</v>
+      </c>
+      <c r="B52">
+        <v>120</v>
+      </c>
+      <c r="C52">
+        <v>50</v>
+      </c>
+      <c r="D52">
+        <v>50</v>
+      </c>
+      <c r="E52">
+        <v>30</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" t="s">
+        <v>12</v>
+      </c>
+      <c r="L52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>0.01</v>
+      </c>
+      <c r="B53">
+        <v>120</v>
+      </c>
+      <c r="C53">
+        <v>120</v>
+      </c>
+      <c r="D53">
+        <v>50</v>
+      </c>
+      <c r="E53">
+        <v>30</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" t="s">
+        <v>12</v>
+      </c>
+      <c r="K53" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A39:K39"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B624D75B-5805-4170-93E2-EB61EBAC6883}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
jaloguin de muchas tareas
</commit_message>
<xml_diff>
--- a/Modelos/Experimentos TFP y STL/Resultados.xlsx
+++ b/Modelos/Experimentos TFP y STL/Resultados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/jd_pradal_uniandes_edu_co/Documents/Documentos/Maestría/Tesis Maestría/Modelos/Experimentos TFP y STL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{34A74DC2-6BF4-4ADA-A2A7-7E00B2D7711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8405A71-C5E7-455D-9BB8-9D60CA80B2BF}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="8_{34A74DC2-6BF4-4ADA-A2A7-7E00B2D7711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85F755C9-390E-4692-BACE-33C9207422D6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{A9FAACA8-E109-4398-B007-65978125D358}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="106">
   <si>
     <t>Nodos 1</t>
   </si>
@@ -209,13 +209,160 @@
   </si>
   <si>
     <t>Contugas TFP Modelo 120 - nodos1 - 120 - nodos2 - 50 Epocas - 2 l2_norm_clip 0.05ruido -0.001  lr -  3 mb -30 Batch</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_r_r_l</t>
+  </si>
+  <si>
+    <t>Activación 1</t>
+  </si>
+  <si>
+    <t>Activación 2</t>
+  </si>
+  <si>
+    <t>Activación 3</t>
+  </si>
+  <si>
+    <t>Relu</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seno_freq_30_amplitud_10_ruido3 </t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_r_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_r_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_r_r_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_r_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_r_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_r_r_t</t>
+  </si>
+  <si>
+    <t>Tanh</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_r_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_r_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_r_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_r_t_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_t_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_t_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_r_t_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_t_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_r_t_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_r_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_r_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_r_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_r_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_r_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_r_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_r_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_r_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_r_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_t_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_t_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_t_r</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_150_n1_150_n2_80_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_t_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_t_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_150_nodos1_150_nodos2_80_Epocas_20_Batch_t_t_t</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_200_n1_200_n2_70_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_200_nodos1_200_nodos2_70_Epocas_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_200_nodos1_200_nodos2_70_Epocas_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 TFP_Modelo_300_n1_300_n2_70_E_2_l2_0.05_ruido_0.001_lr_4_mb_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 Sin ruido_Modelo_300_nodos1_300_nodos2_70_Epocas_20_Batch_t_t_l</t>
+  </si>
+  <si>
+    <t>Seno_freq_30_amplitud_10_ruido3 STL_DP con epsilon0.01_Modelo_300_nodos1_300_nodos2_70_Epocas_20_Batch_t_t_l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +397,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,31 +742,31 @@
   <dimension ref="A3:L53"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K5"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -651,7 +801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5">
         <f>1/100</f>
         <v>0.01</v>
@@ -690,7 +840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6">
         <f>1/100</f>
         <v>0.01</v>
@@ -729,7 +879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7">
         <f>1/100</f>
         <v>0.01</v>
@@ -768,7 +918,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8">
         <f>1/100</f>
         <v>0.01</v>
@@ -807,7 +957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>0.01</v>
       </c>
@@ -845,7 +995,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>0.01</v>
       </c>
@@ -883,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>0.01</v>
       </c>
@@ -921,7 +1071,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>0.01</v>
       </c>
@@ -959,7 +1109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>0.01</v>
       </c>
@@ -997,7 +1147,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>0.01</v>
       </c>
@@ -1035,7 +1185,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>0.01</v>
       </c>
@@ -1073,7 +1223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>0.01</v>
       </c>
@@ -1111,7 +1261,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>0.01</v>
       </c>
@@ -1149,22 +1299,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1199,7 +1349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12">
       <c r="A24">
         <f>1/100</f>
         <v>0.01</v>
@@ -1238,7 +1388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25">
         <f>1/100</f>
         <v>0.01</v>
@@ -1277,7 +1427,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26">
         <f>1/100</f>
         <v>0.01</v>
@@ -1316,7 +1466,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27">
         <f>1/100</f>
         <v>0.01</v>
@@ -1355,7 +1505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>0.01</v>
       </c>
@@ -1393,7 +1543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>0.01</v>
       </c>
@@ -1431,7 +1581,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>0.01</v>
       </c>
@@ -1469,7 +1619,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>0.01</v>
       </c>
@@ -1507,7 +1657,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>0.01</v>
       </c>
@@ -1545,7 +1695,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>0.01</v>
       </c>
@@ -1583,7 +1733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>0.01</v>
       </c>
@@ -1621,7 +1771,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>0.01</v>
       </c>
@@ -1659,7 +1809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>0.01</v>
       </c>
@@ -1697,22 +1847,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:12">
+      <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1747,7 +1897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12">
       <c r="A41">
         <f>1/100</f>
         <v>0.01</v>
@@ -1786,7 +1936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12">
       <c r="A42">
         <f>1/100</f>
         <v>0.01</v>
@@ -1825,7 +1975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12">
       <c r="A43">
         <f>1/100</f>
         <v>0.01</v>
@@ -1864,7 +2014,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12">
       <c r="A44">
         <f>1/100</f>
         <v>0.01</v>
@@ -1903,7 +2053,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>0.01</v>
       </c>
@@ -1941,7 +2091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>0.01</v>
       </c>
@@ -1979,7 +2129,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>0.01</v>
       </c>
@@ -2017,7 +2167,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>0.01</v>
       </c>
@@ -2055,7 +2205,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>0.01</v>
       </c>
@@ -2093,7 +2243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>0.01</v>
       </c>
@@ -2131,7 +2281,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>0.01</v>
       </c>
@@ -2169,7 +2319,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>0.01</v>
       </c>
@@ -2207,7 +2357,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>0.01</v>
       </c>
@@ -2261,27 +2411,27 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:K18"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2316,7 +2466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3">
         <f>1/100</f>
         <v>0.01</v>
@@ -2352,22 +2502,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2402,7 +2552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12">
         <f>1/100</f>
         <v>0.01</v>
@@ -2438,22 +2588,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2488,7 +2638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18">
         <f>1/100</f>
         <v>0.01</v>
@@ -2536,33 +2686,55 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1B16CC-18A0-462A-83C9-A2CEA644640D}">
-  <dimension ref="A3:K20"/>
+  <dimension ref="A2:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2596,8 +2768,17 @@
       <c r="K4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <f>1/100</f>
         <v>0.01</v>
@@ -2609,7 +2790,7 @@
         <v>150</v>
       </c>
       <c r="D5">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -2621,7 +2802,7 @@
         <v>9</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -2632,185 +2813,2119 @@
       <c r="K5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7">
+        <f t="shared" ref="A7:A18" si="0">1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B7">
+        <v>150</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B8">
+        <v>150</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B9">
+        <v>150</v>
+      </c>
+      <c r="C9">
+        <v>150</v>
+      </c>
+      <c r="D9">
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B10">
+        <v>150</v>
+      </c>
+      <c r="C10">
+        <v>150</v>
+      </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" t="s">
+        <v>70</v>
+      </c>
+      <c r="O10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B11">
+        <v>150</v>
+      </c>
+      <c r="C11">
+        <v>150</v>
+      </c>
+      <c r="D11">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B12">
+        <v>150</v>
+      </c>
+      <c r="C12">
+        <v>150</v>
+      </c>
+      <c r="D12">
+        <v>80</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" t="s">
+        <v>61</v>
+      </c>
+      <c r="O12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+      <c r="C13">
+        <v>150</v>
+      </c>
+      <c r="D13">
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B14">
+        <v>150</v>
+      </c>
+      <c r="C14">
+        <v>150</v>
+      </c>
+      <c r="D14">
+        <v>80</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B15">
+        <v>150</v>
+      </c>
+      <c r="C15">
+        <v>150</v>
+      </c>
+      <c r="D15">
+        <v>80</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N15" t="s">
+        <v>61</v>
+      </c>
+      <c r="O15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B16">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16">
+        <v>80</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16" t="s">
+        <v>70</v>
+      </c>
+      <c r="N16" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
+      </c>
+      <c r="D17">
+        <v>70</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" t="s">
+        <v>70</v>
+      </c>
+      <c r="M17" t="s">
+        <v>70</v>
+      </c>
+      <c r="N17" t="s">
+        <v>62</v>
+      </c>
+      <c r="O17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="B18">
+        <v>300</v>
+      </c>
+      <c r="C18">
+        <v>300</v>
+      </c>
+      <c r="D18">
+        <v>70</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" t="s">
+        <v>70</v>
+      </c>
+      <c r="M18" t="s">
+        <v>70</v>
+      </c>
+      <c r="N18" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B26" t="s">
         <v>0</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C26" t="s">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
         <v>5</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H26" t="s">
         <v>10</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I26" t="s">
         <v>6</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J26" t="s">
         <v>7</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="L26" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" t="s">
+        <v>59</v>
+      </c>
+      <c r="N26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
         <f>1/100</f>
         <v>0.01</v>
       </c>
-      <c r="B14">
-        <v>100</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="D14">
+      <c r="B27">
+        <v>150</v>
+      </c>
+      <c r="C27">
+        <v>150</v>
+      </c>
+      <c r="D27">
+        <v>80</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B28">
+        <v>150</v>
+      </c>
+      <c r="C28">
+        <v>150</v>
+      </c>
+      <c r="D28">
+        <v>80</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
+        <f t="shared" ref="A29:A40" si="1">1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B29">
+        <v>150</v>
+      </c>
+      <c r="C29">
+        <v>150</v>
+      </c>
+      <c r="D29">
+        <v>80</v>
+      </c>
+      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M29" t="s">
+        <v>61</v>
+      </c>
+      <c r="N29" t="s">
+        <v>70</v>
+      </c>
+      <c r="O29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B30">
+        <v>150</v>
+      </c>
+      <c r="C30">
+        <v>150</v>
+      </c>
+      <c r="D30">
+        <v>80</v>
+      </c>
+      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30" t="s">
+        <v>70</v>
+      </c>
+      <c r="N30" t="s">
+        <v>62</v>
+      </c>
+      <c r="O30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B31">
+        <v>150</v>
+      </c>
+      <c r="C31">
+        <v>150</v>
+      </c>
+      <c r="D31">
+        <v>80</v>
+      </c>
+      <c r="E31">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31" t="s">
+        <v>70</v>
+      </c>
+      <c r="N31" t="s">
+        <v>61</v>
+      </c>
+      <c r="O31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B32">
+        <v>150</v>
+      </c>
+      <c r="C32">
+        <v>150</v>
+      </c>
+      <c r="D32">
+        <v>80</v>
+      </c>
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" t="s">
+        <v>70</v>
+      </c>
+      <c r="N32" t="s">
+        <v>70</v>
+      </c>
+      <c r="O32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B33">
+        <v>150</v>
+      </c>
+      <c r="C33">
+        <v>150</v>
+      </c>
+      <c r="D33">
+        <v>80</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" t="s">
+        <v>70</v>
+      </c>
+      <c r="M33" t="s">
+        <v>61</v>
+      </c>
+      <c r="N33" t="s">
+        <v>62</v>
+      </c>
+      <c r="O33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B34">
+        <v>150</v>
+      </c>
+      <c r="C34">
+        <v>150</v>
+      </c>
+      <c r="D34">
+        <v>80</v>
+      </c>
+      <c r="E34">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" t="s">
+        <v>70</v>
+      </c>
+      <c r="M34" t="s">
+        <v>61</v>
+      </c>
+      <c r="N34" t="s">
+        <v>61</v>
+      </c>
+      <c r="O34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B35">
+        <v>150</v>
+      </c>
+      <c r="C35">
+        <v>150</v>
+      </c>
+      <c r="D35">
+        <v>80</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" t="s">
+        <v>70</v>
+      </c>
+      <c r="M35" t="s">
+        <v>61</v>
+      </c>
+      <c r="N35" t="s">
+        <v>70</v>
+      </c>
+      <c r="O35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B36">
+        <v>150</v>
+      </c>
+      <c r="C36">
+        <v>150</v>
+      </c>
+      <c r="D36">
+        <v>80</v>
+      </c>
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" t="s">
+        <v>70</v>
+      </c>
+      <c r="M36" t="s">
+        <v>70</v>
+      </c>
+      <c r="N36" t="s">
+        <v>62</v>
+      </c>
+      <c r="O36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B37">
+        <v>150</v>
+      </c>
+      <c r="C37">
+        <v>150</v>
+      </c>
+      <c r="D37">
+        <v>80</v>
+      </c>
+      <c r="E37">
+        <v>20</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" t="s">
+        <v>70</v>
+      </c>
+      <c r="M37" t="s">
+        <v>70</v>
+      </c>
+      <c r="N37" t="s">
+        <v>61</v>
+      </c>
+      <c r="O37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B38">
+        <v>150</v>
+      </c>
+      <c r="C38">
+        <v>150</v>
+      </c>
+      <c r="D38">
+        <v>80</v>
+      </c>
+      <c r="E38">
+        <v>20</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" t="s">
+        <v>70</v>
+      </c>
+      <c r="M38" t="s">
+        <v>70</v>
+      </c>
+      <c r="N38" t="s">
+        <v>70</v>
+      </c>
+      <c r="O38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B39">
+        <v>200</v>
+      </c>
+      <c r="C39">
+        <v>200</v>
+      </c>
+      <c r="D39">
+        <v>70</v>
+      </c>
+      <c r="E39">
+        <v>20</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" t="s">
+        <v>70</v>
+      </c>
+      <c r="M39" t="s">
+        <v>70</v>
+      </c>
+      <c r="N39" t="s">
+        <v>62</v>
+      </c>
+      <c r="O39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="B40">
+        <v>300</v>
+      </c>
+      <c r="C40">
+        <v>300</v>
+      </c>
+      <c r="D40">
+        <v>70</v>
+      </c>
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" t="s">
+        <v>12</v>
+      </c>
+      <c r="K40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" t="s">
+        <v>70</v>
+      </c>
+      <c r="M40" t="s">
+        <v>70</v>
+      </c>
+      <c r="N40" t="s">
+        <v>62</v>
+      </c>
+      <c r="O40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" t="s">
         <v>10</v>
       </c>
-      <c r="E14">
-        <v>30</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="I44" t="s">
         <v>6</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J44" t="s">
         <v>7</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K44" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="L44" t="s">
+        <v>58</v>
+      </c>
+      <c r="M44" t="s">
+        <v>59</v>
+      </c>
+      <c r="N44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45">
         <f>1/100</f>
         <v>0.01</v>
       </c>
-      <c r="B20">
-        <v>100</v>
-      </c>
-      <c r="C20">
-        <v>100</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <v>30</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="I20" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" t="s">
-        <v>12</v>
+      <c r="B45">
+        <v>150</v>
+      </c>
+      <c r="C45">
+        <v>150</v>
+      </c>
+      <c r="D45">
+        <v>80</v>
+      </c>
+      <c r="E45">
+        <v>20</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" t="s">
+        <v>61</v>
+      </c>
+      <c r="M45" t="s">
+        <v>61</v>
+      </c>
+      <c r="N45" t="s">
+        <v>62</v>
+      </c>
+      <c r="O45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B46">
+        <v>150</v>
+      </c>
+      <c r="C46">
+        <v>150</v>
+      </c>
+      <c r="D46">
+        <v>80</v>
+      </c>
+      <c r="E46">
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" t="s">
+        <v>61</v>
+      </c>
+      <c r="M46" t="s">
+        <v>61</v>
+      </c>
+      <c r="N46" t="s">
+        <v>61</v>
+      </c>
+      <c r="O46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47">
+        <f t="shared" ref="A47:A58" si="2">1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B47">
+        <v>150</v>
+      </c>
+      <c r="C47">
+        <v>150</v>
+      </c>
+      <c r="D47">
+        <v>80</v>
+      </c>
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47">
+        <v>4</v>
+      </c>
+      <c r="I47" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" t="s">
+        <v>61</v>
+      </c>
+      <c r="M47" t="s">
+        <v>61</v>
+      </c>
+      <c r="N47" t="s">
+        <v>70</v>
+      </c>
+      <c r="O47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B48">
+        <v>150</v>
+      </c>
+      <c r="C48">
+        <v>150</v>
+      </c>
+      <c r="D48">
+        <v>80</v>
+      </c>
+      <c r="E48">
+        <v>20</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+      <c r="I48" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" t="s">
+        <v>12</v>
+      </c>
+      <c r="K48" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" t="s">
+        <v>61</v>
+      </c>
+      <c r="M48" t="s">
+        <v>70</v>
+      </c>
+      <c r="N48" t="s">
+        <v>62</v>
+      </c>
+      <c r="O48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B49">
+        <v>150</v>
+      </c>
+      <c r="C49">
+        <v>150</v>
+      </c>
+      <c r="D49">
+        <v>80</v>
+      </c>
+      <c r="E49">
+        <v>20</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
+      <c r="I49" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49" t="s">
+        <v>12</v>
+      </c>
+      <c r="L49" t="s">
+        <v>61</v>
+      </c>
+      <c r="M49" t="s">
+        <v>70</v>
+      </c>
+      <c r="N49" t="s">
+        <v>61</v>
+      </c>
+      <c r="O49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B50">
+        <v>150</v>
+      </c>
+      <c r="C50">
+        <v>150</v>
+      </c>
+      <c r="D50">
+        <v>80</v>
+      </c>
+      <c r="E50">
+        <v>20</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H50">
+        <v>4</v>
+      </c>
+      <c r="I50" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" t="s">
+        <v>12</v>
+      </c>
+      <c r="K50" t="s">
+        <v>12</v>
+      </c>
+      <c r="L50" t="s">
+        <v>61</v>
+      </c>
+      <c r="M50" t="s">
+        <v>70</v>
+      </c>
+      <c r="N50" t="s">
+        <v>70</v>
+      </c>
+      <c r="O50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B51">
+        <v>150</v>
+      </c>
+      <c r="C51">
+        <v>150</v>
+      </c>
+      <c r="D51">
+        <v>80</v>
+      </c>
+      <c r="E51">
+        <v>20</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51">
+        <v>4</v>
+      </c>
+      <c r="I51" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" t="s">
+        <v>70</v>
+      </c>
+      <c r="M51" t="s">
+        <v>61</v>
+      </c>
+      <c r="N51" t="s">
+        <v>62</v>
+      </c>
+      <c r="O51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B52">
+        <v>150</v>
+      </c>
+      <c r="C52">
+        <v>150</v>
+      </c>
+      <c r="D52">
+        <v>80</v>
+      </c>
+      <c r="E52">
+        <v>20</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+      <c r="I52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" t="s">
+        <v>12</v>
+      </c>
+      <c r="L52" t="s">
+        <v>70</v>
+      </c>
+      <c r="M52" t="s">
+        <v>61</v>
+      </c>
+      <c r="N52" t="s">
+        <v>61</v>
+      </c>
+      <c r="O52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B53">
+        <v>150</v>
+      </c>
+      <c r="C53">
+        <v>150</v>
+      </c>
+      <c r="D53">
+        <v>80</v>
+      </c>
+      <c r="E53">
+        <v>20</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+      <c r="I53" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" t="s">
+        <v>12</v>
+      </c>
+      <c r="K53" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" t="s">
+        <v>70</v>
+      </c>
+      <c r="M53" t="s">
+        <v>61</v>
+      </c>
+      <c r="N53" t="s">
+        <v>70</v>
+      </c>
+      <c r="O53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B54">
+        <v>150</v>
+      </c>
+      <c r="C54">
+        <v>150</v>
+      </c>
+      <c r="D54">
+        <v>80</v>
+      </c>
+      <c r="E54">
+        <v>20</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54">
+        <v>4</v>
+      </c>
+      <c r="I54" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" t="s">
+        <v>12</v>
+      </c>
+      <c r="K54" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" t="s">
+        <v>70</v>
+      </c>
+      <c r="M54" t="s">
+        <v>70</v>
+      </c>
+      <c r="N54" t="s">
+        <v>62</v>
+      </c>
+      <c r="O54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B55">
+        <v>150</v>
+      </c>
+      <c r="C55">
+        <v>150</v>
+      </c>
+      <c r="D55">
+        <v>80</v>
+      </c>
+      <c r="E55">
+        <v>20</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+      <c r="I55" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" t="s">
+        <v>12</v>
+      </c>
+      <c r="K55" t="s">
+        <v>12</v>
+      </c>
+      <c r="L55" t="s">
+        <v>70</v>
+      </c>
+      <c r="M55" t="s">
+        <v>70</v>
+      </c>
+      <c r="N55" t="s">
+        <v>61</v>
+      </c>
+      <c r="O55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B56">
+        <v>150</v>
+      </c>
+      <c r="C56">
+        <v>150</v>
+      </c>
+      <c r="D56">
+        <v>80</v>
+      </c>
+      <c r="E56">
+        <v>20</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
+      <c r="I56" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" t="s">
+        <v>12</v>
+      </c>
+      <c r="K56" t="s">
+        <v>12</v>
+      </c>
+      <c r="L56" t="s">
+        <v>70</v>
+      </c>
+      <c r="M56" t="s">
+        <v>70</v>
+      </c>
+      <c r="N56" t="s">
+        <v>70</v>
+      </c>
+      <c r="O56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B57">
+        <v>200</v>
+      </c>
+      <c r="C57">
+        <v>200</v>
+      </c>
+      <c r="D57">
+        <v>70</v>
+      </c>
+      <c r="E57">
+        <v>20</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57" t="s">
+        <v>9</v>
+      </c>
+      <c r="H57">
+        <v>4</v>
+      </c>
+      <c r="I57" t="s">
+        <v>11</v>
+      </c>
+      <c r="J57" t="s">
+        <v>12</v>
+      </c>
+      <c r="K57" t="s">
+        <v>12</v>
+      </c>
+      <c r="L57" t="s">
+        <v>70</v>
+      </c>
+      <c r="M57" t="s">
+        <v>70</v>
+      </c>
+      <c r="N57" t="s">
+        <v>62</v>
+      </c>
+      <c r="O57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="B58">
+        <v>300</v>
+      </c>
+      <c r="C58">
+        <v>300</v>
+      </c>
+      <c r="D58">
+        <v>70</v>
+      </c>
+      <c r="E58">
+        <v>20</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58">
+        <v>4</v>
+      </c>
+      <c r="I58" t="s">
+        <v>11</v>
+      </c>
+      <c r="J58" t="s">
+        <v>12</v>
+      </c>
+      <c r="K58" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" t="s">
+        <v>70</v>
+      </c>
+      <c r="M58" t="s">
+        <v>70</v>
+      </c>
+      <c r="N58" t="s">
+        <v>62</v>
+      </c>
+      <c r="O58" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A2:N2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>